<commit_message>
Species Analysis, SIMPER, indicspecies
</commit_message>
<xml_diff>
--- a/SIMPER_data.xlsx
+++ b/SIMPER_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17193\Downloads\salvador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FF954AA0-D5E1-4B57-AEB4-0A56FD57725E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1A1135-406E-4ABD-8F4A-E62B1A1EEEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Influential Species" sheetId="2" r:id="rId1"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1106,10 +1106,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -3634,11 +3634,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5572,7 +5572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7607,7 +7607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9651,7 +9651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">

</xml_diff>